<commit_message>
Update mapping.xlsx with revised data entries
</commit_message>
<xml_diff>
--- a/mapping.xlsx
+++ b/mapping.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\8. Private\Tool\demowinformapp\demowinformapp\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E266D55D-E06A-44C8-AFC0-A28AF763DF7D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B0479640-435D-472B-AE03-A1C1D9CA5561}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1647" uniqueCount="285">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1649" uniqueCount="287">
   <si>
     <t>TABLE_NAME</t>
   </si>
@@ -852,12 +852,6 @@
     <t>HISSU</t>
   </si>
   <si>
-    <t>TIME_STAMP</t>
-  </si>
-  <si>
-    <t>timestamp</t>
-  </si>
-  <si>
     <t>T_KIHON_PJ_ICHIRAN</t>
     <phoneticPr fontId="1"/>
   </si>
@@ -923,6 +917,22 @@
   </si>
   <si>
     <t>SHITEI_NASHI</t>
+  </si>
+  <si>
+    <t>B</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>E</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>BL</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>T_KIHON_PJ_HYOUJI</t>
+    <phoneticPr fontId="1"/>
   </si>
 </sst>
 </file>
@@ -1251,10 +1261,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:H313"/>
+  <dimension ref="A1:H312"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A286" workbookViewId="0">
-      <selection activeCell="D297" sqref="D297"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="J4" sqref="J4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="21.58203125" defaultRowHeight="18"/>
@@ -3975,7 +3985,7 @@
     </row>
     <row r="136" spans="1:8">
       <c r="A136" s="2" t="s">
-        <v>271</v>
+        <v>269</v>
       </c>
       <c r="B136" t="s">
         <v>9</v>
@@ -4018,7 +4028,7 @@
         <v>167</v>
       </c>
       <c r="B138" t="s">
-        <v>272</v>
+        <v>270</v>
       </c>
       <c r="C138" t="s">
         <v>66</v>
@@ -4255,7 +4265,7 @@
     </row>
     <row r="150" spans="1:8">
       <c r="A150" s="2" t="s">
-        <v>271</v>
+        <v>269</v>
       </c>
       <c r="B150" t="s">
         <v>162</v>
@@ -6358,7 +6368,7 @@
     </row>
     <row r="255" spans="1:8">
       <c r="A255" s="2" t="s">
-        <v>269</v>
+        <v>267</v>
       </c>
       <c r="B255" t="s">
         <v>9</v>
@@ -6401,7 +6411,7 @@
         <v>222</v>
       </c>
       <c r="B257" t="s">
-        <v>270</v>
+        <v>268</v>
       </c>
       <c r="C257" t="s">
         <v>66</v>
@@ -7038,7 +7048,7 @@
     </row>
     <row r="289" spans="1:8">
       <c r="A289" s="2" t="s">
-        <v>267</v>
+        <v>265</v>
       </c>
       <c r="B289" t="s">
         <v>9</v>
@@ -7078,10 +7088,10 @@
     </row>
     <row r="291" spans="1:8">
       <c r="A291" s="2" t="s">
-        <v>267</v>
+        <v>265</v>
       </c>
       <c r="B291" t="s">
-        <v>268</v>
+        <v>266</v>
       </c>
       <c r="C291" t="s">
         <v>66</v>
@@ -7093,7 +7103,7 @@
         <v>12</v>
       </c>
       <c r="F291" t="s">
-        <v>279</v>
+        <v>277</v>
       </c>
     </row>
     <row r="292" spans="1:8">
@@ -7193,7 +7203,7 @@
         <v>16</v>
       </c>
       <c r="H296" t="s">
-        <v>273</v>
+        <v>271</v>
       </c>
     </row>
     <row r="297" spans="1:8">
@@ -7213,7 +7223,7 @@
         <v>16</v>
       </c>
       <c r="H297" t="s">
-        <v>274</v>
+        <v>272</v>
       </c>
     </row>
     <row r="298" spans="1:8">
@@ -7233,7 +7243,7 @@
         <v>16</v>
       </c>
       <c r="H298" t="s">
-        <v>275</v>
+        <v>273</v>
       </c>
     </row>
     <row r="299" spans="1:8">
@@ -7253,7 +7263,7 @@
         <v>16</v>
       </c>
       <c r="H299" t="s">
-        <v>276</v>
+        <v>274</v>
       </c>
     </row>
     <row r="300" spans="1:8">
@@ -7273,7 +7283,7 @@
         <v>16</v>
       </c>
       <c r="H300" t="s">
-        <v>277</v>
+        <v>275</v>
       </c>
     </row>
     <row r="301" spans="1:8">
@@ -7293,7 +7303,7 @@
         <v>16</v>
       </c>
       <c r="H301" t="s">
-        <v>278</v>
+        <v>276</v>
       </c>
     </row>
     <row r="302" spans="1:8">
@@ -7337,8 +7347,8 @@
       </c>
     </row>
     <row r="304" spans="1:8">
-      <c r="A304" t="s">
-        <v>280</v>
+      <c r="A304" s="2" t="s">
+        <v>286</v>
       </c>
       <c r="B304" t="s">
         <v>9</v>
@@ -7352,10 +7362,13 @@
       <c r="E304" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="305" spans="1:5">
-      <c r="A305" t="s">
-        <v>280</v>
+      <c r="F304" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="305" spans="1:8">
+      <c r="A305" s="2" t="s">
+        <v>278</v>
       </c>
       <c r="B305" t="s">
         <v>65</v>
@@ -7369,13 +7382,16 @@
       <c r="E305" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="306" spans="1:5">
-      <c r="A306" t="s">
-        <v>280</v>
+      <c r="F305" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="306" spans="1:8">
+      <c r="A306" s="2" t="s">
+        <v>278</v>
       </c>
       <c r="B306" t="s">
-        <v>281</v>
+        <v>279</v>
       </c>
       <c r="C306" t="s">
         <v>66</v>
@@ -7386,10 +7402,13 @@
       <c r="E306" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="307" spans="1:5">
-      <c r="A307" t="s">
-        <v>280</v>
+      <c r="F306" t="s">
+        <v>277</v>
+      </c>
+    </row>
+    <row r="307" spans="1:8">
+      <c r="A307" s="2" t="s">
+        <v>278</v>
       </c>
       <c r="B307" t="s">
         <v>135</v>
@@ -7403,13 +7422,16 @@
       <c r="E307" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="308" spans="1:5">
-      <c r="A308" t="s">
+      <c r="F307">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="308" spans="1:8">
+      <c r="A308" s="2" t="s">
+        <v>278</v>
+      </c>
+      <c r="B308" t="s">
         <v>280</v>
-      </c>
-      <c r="B308" t="s">
-        <v>282</v>
       </c>
       <c r="C308" t="s">
         <v>15</v>
@@ -7420,13 +7442,16 @@
       <c r="E308" t="s">
         <v>16</v>
       </c>
-    </row>
-    <row r="309" spans="1:5">
-      <c r="A309" t="s">
-        <v>280</v>
+      <c r="H308" t="s">
+        <v>283</v>
+      </c>
+    </row>
+    <row r="309" spans="1:8">
+      <c r="A309" s="2" t="s">
+        <v>278</v>
       </c>
       <c r="B309" t="s">
-        <v>283</v>
+        <v>281</v>
       </c>
       <c r="C309" t="s">
         <v>15</v>
@@ -7437,13 +7462,16 @@
       <c r="E309" t="s">
         <v>16</v>
       </c>
-    </row>
-    <row r="310" spans="1:5">
-      <c r="A310" t="s">
-        <v>280</v>
+      <c r="H309" t="s">
+        <v>284</v>
+      </c>
+    </row>
+    <row r="310" spans="1:8">
+      <c r="A310" s="2" t="s">
+        <v>278</v>
       </c>
       <c r="B310" t="s">
-        <v>284</v>
+        <v>282</v>
       </c>
       <c r="C310" t="s">
         <v>15</v>
@@ -7454,56 +7482,48 @@
       <c r="E310" t="s">
         <v>16</v>
       </c>
-    </row>
-    <row r="311" spans="1:5">
-      <c r="A311" t="s">
-        <v>280</v>
+      <c r="H310" t="s">
+        <v>285</v>
+      </c>
+    </row>
+    <row r="311" spans="1:8">
+      <c r="A311" s="2" t="s">
+        <v>278</v>
       </c>
       <c r="B311" t="s">
-        <v>265</v>
+        <v>161</v>
       </c>
       <c r="C311" t="s">
-        <v>266</v>
+        <v>24</v>
       </c>
       <c r="D311" t="s">
         <v>11</v>
       </c>
       <c r="E311" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="312" spans="1:5">
-      <c r="A312" t="s">
-        <v>280</v>
+        <v>16</v>
+      </c>
+      <c r="F311" t="s">
+        <v>277</v>
+      </c>
+    </row>
+    <row r="312" spans="1:8">
+      <c r="A312" s="2" t="s">
+        <v>278</v>
       </c>
       <c r="B312" t="s">
-        <v>161</v>
+        <v>162</v>
       </c>
       <c r="C312" t="s">
-        <v>24</v>
+        <v>56</v>
       </c>
       <c r="D312" t="s">
         <v>11</v>
       </c>
       <c r="E312" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="313" spans="1:5">
-      <c r="A313" t="s">
-        <v>280</v>
-      </c>
-      <c r="B313" t="s">
-        <v>162</v>
-      </c>
-      <c r="C313" t="s">
-        <v>56</v>
-      </c>
-      <c r="D313" t="s">
-        <v>11</v>
-      </c>
-      <c r="E313" t="s">
-        <v>12</v>
+        <v>12</v>
+      </c>
+      <c r="F312">
+        <v>0</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Add processing for T_KIHON_PJ_HYOUJI and update key order in JSON export
</commit_message>
<xml_diff>
--- a/mapping.xlsx
+++ b/mapping.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\8. Private\Tool\demowinformapp\demowinformapp\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B0479640-435D-472B-AE03-A1C1D9CA5561}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5F781510-2181-45E7-BD12-B75E0C8888EE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1649" uniqueCount="287">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1649" uniqueCount="288">
   <si>
     <t>TABLE_NAME</t>
   </si>
@@ -932,6 +932,10 @@
   </si>
   <si>
     <t>T_KIHON_PJ_HYOUJI</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>T_KIHON_PJ_GAMEN</t>
     <phoneticPr fontId="1"/>
   </si>
 </sst>
@@ -1263,8 +1267,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:H312"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J4" sqref="J4"/>
+    <sheetView tabSelected="1" topLeftCell="A295" workbookViewId="0">
+      <selection activeCell="D305" sqref="D305"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="21.58203125" defaultRowHeight="18"/>
@@ -1945,7 +1949,7 @@
     </row>
     <row r="34" spans="1:7">
       <c r="A34" s="2" t="s">
-        <v>63</v>
+        <v>287</v>
       </c>
       <c r="B34" t="s">
         <v>9</v>

</xml_diff>

<commit_message>
Add initial version of the game document (doc_gamen.xlsx)
</commit_message>
<xml_diff>
--- a/mapping.xlsx
+++ b/mapping.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\8. Private\Tool\demowinformapp\demowinformapp\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5F781510-2181-45E7-BD12-B75E0C8888EE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{904D0A2B-4786-4BAE-BD0D-D28AD53F01D9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1649" uniqueCount="288">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1649" uniqueCount="294">
   <si>
     <t>TABLE_NAME</t>
   </si>
@@ -936,6 +936,30 @@
   </si>
   <si>
     <t>T_KIHON_PJ_GAMEN</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>T_KIHON_PJ_HYOUJI</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>T_KIHON_PJ_KOUMOKU</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>T_KIHON_PJ_KOUMOKU_LOGIC</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>T_KIHON_PJ_KOUMOKU_CSV</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>T_KIHON_PJ_IPO</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>T_KIHON_PJ_MENU</t>
     <phoneticPr fontId="1"/>
   </si>
 </sst>
@@ -1267,8 +1291,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:H312"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A295" workbookViewId="0">
-      <selection activeCell="D305" sqref="D305"/>
+    <sheetView tabSelected="1" topLeftCell="A300" workbookViewId="0">
+      <selection activeCell="I311" sqref="I311"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="21.58203125" defaultRowHeight="18"/>
@@ -4229,7 +4253,7 @@
     </row>
     <row r="148" spans="1:8">
       <c r="A148" s="2" t="s">
-        <v>167</v>
+        <v>292</v>
       </c>
       <c r="B148" t="s">
         <v>43</v>
@@ -4309,7 +4333,7 @@
     </row>
     <row r="152" spans="1:8">
       <c r="A152" s="2" t="s">
-        <v>180</v>
+        <v>289</v>
       </c>
       <c r="B152" t="s">
         <v>9</v>
@@ -4852,7 +4876,7 @@
     </row>
     <row r="179" spans="1:8">
       <c r="A179" s="2" t="s">
-        <v>205</v>
+        <v>290</v>
       </c>
       <c r="B179" t="s">
         <v>9</v>
@@ -5252,7 +5276,7 @@
     </row>
     <row r="199" spans="1:8">
       <c r="A199" s="2" t="s">
-        <v>208</v>
+        <v>291</v>
       </c>
       <c r="B199" t="s">
         <v>154</v>
@@ -6452,7 +6476,7 @@
     </row>
     <row r="259" spans="1:8">
       <c r="A259" s="2" t="s">
-        <v>222</v>
+        <v>293</v>
       </c>
       <c r="B259" t="s">
         <v>136</v>
@@ -7166,7 +7190,7 @@
       <c r="E294" t="s">
         <v>16</v>
       </c>
-      <c r="G294">
+      <c r="F294">
         <v>999999</v>
       </c>
     </row>
@@ -7512,7 +7536,7 @@
     </row>
     <row r="312" spans="1:8">
       <c r="A312" s="2" t="s">
-        <v>278</v>
+        <v>288</v>
       </c>
       <c r="B312" t="s">
         <v>162</v>

</xml_diff>